<commit_message>
Buildings chosen for D5.2
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE5793DD-17A9-4EC6-A98C-FC9C1C5909AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A36235-1F08-4B2B-9C0E-EB496BF2CF0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OperationScenario_Component_Bui!$A$1:$P$17</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>ID_Building</t>
   </si>
@@ -72,14 +75,11 @@
   <si>
     <t>SFH</t>
   </si>
-  <si>
-    <t>MFH</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +394,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -557,8 +563,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,12 +921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -970,107 +985,808 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>1880</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1918</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>183.79400000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>270.53500000000003</v>
+      </c>
+      <c r="H2" s="2">
+        <v>102.03</v>
+      </c>
+      <c r="I2" s="2">
+        <v>51.991999999999997</v>
+      </c>
+      <c r="J2" s="2">
+        <v>398415.375</v>
+      </c>
+      <c r="K2" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="L2" s="2">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2">
+        <v>7.4429999999999996</v>
+      </c>
+      <c r="N2" s="2">
+        <v>4.8940000000000001</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1.371</v>
+      </c>
+      <c r="P2" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1979</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1983</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>185.137</v>
+      </c>
+      <c r="G3" s="2">
+        <v>214.91200000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>90.760999999999996</v>
+      </c>
+      <c r="I3" s="2">
+        <v>52.371000000000002</v>
+      </c>
+      <c r="J3" s="2">
+        <v>213505.516</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3</v>
+      </c>
+      <c r="M3" s="2">
+        <v>8.3230000000000004</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5.5490000000000004</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1.5409999999999999</v>
+      </c>
+      <c r="P3" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1995</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>177.626</v>
+      </c>
+      <c r="G4" s="2">
+        <v>98.600999999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>104.66800000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>50.247</v>
+      </c>
+      <c r="J4" s="2">
+        <v>213505.516</v>
+      </c>
+      <c r="K4" s="2">
+        <v>3</v>
+      </c>
+      <c r="L4" s="2">
+        <v>3</v>
+      </c>
+      <c r="M4" s="2">
+        <v>15.365</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5.5869999999999997</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2.3279999999999998</v>
+      </c>
+      <c r="P4" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
         <v>2002</v>
       </c>
-      <c r="D2">
-        <v>2008</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>168.32</v>
-      </c>
-      <c r="G2">
-        <v>226.23599999999999</v>
-      </c>
-      <c r="H2">
-        <v>156.036</v>
-      </c>
-      <c r="I2">
-        <v>47.613999999999997</v>
-      </c>
-      <c r="J2">
+      <c r="D5" s="2">
+        <v>2004</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>176.86099999999999</v>
+      </c>
+      <c r="G5" s="2">
+        <v>95.753</v>
+      </c>
+      <c r="H5" s="2">
+        <v>64.212000000000003</v>
+      </c>
+      <c r="I5" s="2">
+        <v>50.030999999999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L5" s="2">
+        <v>3</v>
+      </c>
+      <c r="M5" s="2">
+        <v>8.452</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3.6219999999999999</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1.3420000000000001</v>
+      </c>
+      <c r="P5" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>177.167</v>
+      </c>
+      <c r="G6" s="2">
+        <v>100.527</v>
+      </c>
+      <c r="H6" s="2">
+        <v>61.503999999999998</v>
+      </c>
+      <c r="I6" s="2">
+        <v>55.128999999999998</v>
+      </c>
+      <c r="J6" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L6" s="2">
+        <v>3</v>
+      </c>
+      <c r="M6" s="2">
+        <v>7.9589999999999996</v>
+      </c>
+      <c r="N6" s="2">
+        <v>3.411</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1.2629999999999999</v>
+      </c>
+      <c r="P6" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2007</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>169.459</v>
+      </c>
+      <c r="G7" s="2">
+        <v>94.391999999999996</v>
+      </c>
+      <c r="H7" s="2">
+        <v>62.491</v>
+      </c>
+      <c r="I7" s="2">
+        <v>52.73</v>
+      </c>
+      <c r="J7" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L7" s="2">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2">
+        <v>8.2070000000000007</v>
+      </c>
+      <c r="N7" s="2">
+        <v>3.5169999999999999</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1.3029999999999999</v>
+      </c>
+      <c r="P7" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1919</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1948</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>166.934</v>
+      </c>
+      <c r="G8" s="2">
+        <v>223.42500000000001</v>
+      </c>
+      <c r="H8" s="2">
+        <v>130.68299999999999</v>
+      </c>
+      <c r="I8" s="2">
+        <v>47.222000000000001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>338121.65600000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="L8" s="2">
+        <v>3</v>
+      </c>
+      <c r="M8" s="2">
+        <v>12.082000000000001</v>
+      </c>
+      <c r="N8" s="2">
+        <v>5.7439999999999998</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1.9810000000000001</v>
+      </c>
+      <c r="P8" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1949</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1957</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>174.14</v>
+      </c>
+      <c r="G9" s="2">
+        <v>273.15499999999997</v>
+      </c>
+      <c r="H9" s="2">
+        <v>114.283</v>
+      </c>
+      <c r="I9" s="2">
+        <v>49.261000000000003</v>
+      </c>
+      <c r="J9" s="2">
         <v>213505.516</v>
       </c>
-      <c r="K2">
-        <v>3</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
-      </c>
-      <c r="M2">
-        <v>10.483000000000001</v>
-      </c>
-      <c r="N2">
-        <v>4.3680000000000003</v>
-      </c>
-      <c r="O2">
-        <v>2.621</v>
-      </c>
-      <c r="P2">
+      <c r="K9" s="2">
+        <v>3</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>10.037000000000001</v>
+      </c>
+      <c r="N9" s="2">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1.619</v>
+      </c>
+      <c r="P9" s="1">
         <v>21000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3">
-        <v>2002</v>
-      </c>
-      <c r="D3">
-        <v>2008</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>894.928</v>
-      </c>
-      <c r="G3">
-        <v>684.21</v>
-      </c>
-      <c r="H3">
-        <v>462.03500000000003</v>
-      </c>
-      <c r="I3">
-        <v>253.15700000000001</v>
-      </c>
-      <c r="J3">
+    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1958</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1968</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2">
+        <v>175.60900000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>302.37900000000002</v>
+      </c>
+      <c r="H10" s="2">
+        <v>155.72800000000001</v>
+      </c>
+      <c r="I10" s="2">
+        <v>49.676000000000002</v>
+      </c>
+      <c r="J10" s="2">
         <v>213505.516</v>
       </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>3</v>
-      </c>
-      <c r="M3">
-        <v>30.928999999999998</v>
-      </c>
-      <c r="N3">
-        <v>12.887</v>
-      </c>
-      <c r="O3">
-        <v>7.7320000000000002</v>
-      </c>
-      <c r="P3">
-        <v>2100000</v>
+      <c r="K10" s="2">
+        <v>3</v>
+      </c>
+      <c r="L10" s="2">
+        <v>3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>13.315</v>
+      </c>
+      <c r="N10" s="2">
+        <v>7.7089999999999996</v>
+      </c>
+      <c r="O10" s="2">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="P10" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>47</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1969</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1978</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>184.14500000000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>270.49700000000001</v>
+      </c>
+      <c r="H11" s="2">
+        <v>150.87700000000001</v>
+      </c>
+      <c r="I11" s="2">
+        <v>52.091000000000001</v>
+      </c>
+      <c r="J11" s="2">
+        <v>213505.516</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3</v>
+      </c>
+      <c r="M11" s="2">
+        <v>14.753</v>
+      </c>
+      <c r="N11" s="2">
+        <v>5.9930000000000003</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2.3050000000000002</v>
+      </c>
+      <c r="P11" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1994</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>182.928</v>
+      </c>
+      <c r="G12" s="2">
+        <v>145.40700000000001</v>
+      </c>
+      <c r="H12" s="2">
+        <v>123.01900000000001</v>
+      </c>
+      <c r="I12" s="2">
+        <v>51.747</v>
+      </c>
+      <c r="J12" s="2">
+        <v>213505.516</v>
+      </c>
+      <c r="K12" s="2">
+        <v>3</v>
+      </c>
+      <c r="L12" s="2">
+        <v>3</v>
+      </c>
+      <c r="M12" s="2">
+        <v>13.516999999999999</v>
+      </c>
+      <c r="N12" s="2">
+        <v>8.2070000000000007</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2.4140000000000001</v>
+      </c>
+      <c r="P12" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2006</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>186.50299999999999</v>
+      </c>
+      <c r="G13" s="2">
+        <v>99.061000000000007</v>
+      </c>
+      <c r="H13" s="2">
+        <v>62.307000000000002</v>
+      </c>
+      <c r="I13" s="2">
+        <v>58.033999999999999</v>
+      </c>
+      <c r="J13" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L13" s="2">
+        <v>3</v>
+      </c>
+      <c r="M13" s="2">
+        <v>8.7889999999999997</v>
+      </c>
+      <c r="N13" s="2">
+        <v>3.7669999999999999</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1.395</v>
+      </c>
+      <c r="P13" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2012</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>214.02799999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>110.389</v>
+      </c>
+      <c r="H14" s="2">
+        <v>64.798000000000002</v>
+      </c>
+      <c r="I14" s="2">
+        <v>66.599000000000004</v>
+      </c>
+      <c r="J14" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L14" s="2">
+        <v>3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>9.5169999999999995</v>
+      </c>
+      <c r="N14" s="2">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="P14" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2012</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>155.95400000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>87.111000000000004</v>
+      </c>
+      <c r="H15" s="2">
+        <v>49.99</v>
+      </c>
+      <c r="I15" s="2">
+        <v>48.527999999999999</v>
+      </c>
+      <c r="J15" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L15" s="2">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2">
+        <v>7.86</v>
+      </c>
+      <c r="N15" s="2">
+        <v>3.3679999999999999</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.248</v>
+      </c>
+      <c r="P15" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>214.02799999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <v>96.319000000000003</v>
+      </c>
+      <c r="H16" s="2">
+        <v>59.613</v>
+      </c>
+      <c r="I16" s="2">
+        <v>66.599000000000004</v>
+      </c>
+      <c r="J16" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2">
+        <v>9.5169999999999995</v>
+      </c>
+      <c r="N16" s="2">
+        <v>4.0789999999999997</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.5109999999999999</v>
+      </c>
+      <c r="P16" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>78</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>155.95400000000001</v>
+      </c>
+      <c r="G17" s="2">
+        <v>75.715000000000003</v>
+      </c>
+      <c r="H17" s="2">
+        <v>48.85</v>
+      </c>
+      <c r="I17" s="2">
+        <v>48.527999999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>148226.875</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3</v>
+      </c>
+      <c r="M17" s="2">
+        <v>7.86</v>
+      </c>
+      <c r="N17" s="2">
+        <v>3.3679999999999999</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1.248</v>
+      </c>
+      <c r="P17" s="1">
+        <v>21000</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P17" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
two groups (5B2EP and 3B1EP) of scenarios are run
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE701FE4-E370-FD42-ABBD-ED00616B0811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85998DD4-A045-DA44-BBC4-71B1DCA3CB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="-18060" windowWidth="25880" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OperationScenario_Component_Bui!$A$1:$P$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OperationScenario_Component_Bui!$A$1:$P$4</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>ID_Building</t>
   </si>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,7 +980,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -998,10 +998,10 @@
         <v>174.14</v>
       </c>
       <c r="G2" s="1">
-        <v>303.87599999999998</v>
+        <v>286.52800000000002</v>
       </c>
       <c r="H2" s="1">
-        <v>117.355</v>
+        <v>115.621</v>
       </c>
       <c r="I2" s="1">
         <v>49.261000000000003</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -1048,10 +1048,10 @@
         <v>174.14</v>
       </c>
       <c r="G3" s="1">
-        <v>286.52800000000002</v>
+        <v>273.15499999999997</v>
       </c>
       <c r="H3" s="1">
-        <v>115.621</v>
+        <v>114.283</v>
       </c>
       <c r="I3" s="1">
         <v>49.261000000000003</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1098,10 +1098,10 @@
         <v>174.14</v>
       </c>
       <c r="G4" s="1">
-        <v>274.81700000000001</v>
+        <v>303.87599999999998</v>
       </c>
       <c r="H4" s="1">
-        <v>114.45</v>
+        <v>136.28700000000001</v>
       </c>
       <c r="I4" s="1">
         <v>49.261000000000003</v>
@@ -1128,109 +1128,9 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1949</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1957</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1">
-        <v>174.14</v>
-      </c>
-      <c r="G5" s="1">
-        <v>273.15499999999997</v>
-      </c>
-      <c r="H5" s="1">
-        <v>114.283</v>
-      </c>
-      <c r="I5" s="1">
-        <v>49.261000000000003</v>
-      </c>
-      <c r="J5" s="1">
-        <v>213505.516</v>
-      </c>
-      <c r="K5" s="1">
-        <v>3</v>
-      </c>
-      <c r="L5" s="1">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
-        <v>10.037000000000001</v>
-      </c>
-      <c r="N5" s="1">
-        <v>4.5330000000000004</v>
-      </c>
-      <c r="O5" s="1">
-        <v>1.619</v>
-      </c>
-      <c r="P5" s="1">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1949</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1957</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>174.14</v>
-      </c>
-      <c r="G6" s="1">
-        <v>303.87599999999998</v>
-      </c>
-      <c r="H6" s="1">
-        <v>136.28700000000001</v>
-      </c>
-      <c r="I6" s="1">
-        <v>49.261000000000003</v>
-      </c>
-      <c r="J6" s="1">
-        <v>213505.516</v>
-      </c>
-      <c r="K6" s="1">
-        <v>3</v>
-      </c>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="M6" s="1">
-        <v>10.037000000000001</v>
-      </c>
-      <c r="N6" s="1">
-        <v>4.5330000000000004</v>
-      </c>
-      <c r="O6" s="1">
-        <v>1.619</v>
-      </c>
-      <c r="P6" s="1">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:P6" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
+  <autoFilter ref="A1:P4" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AlwaysCooling scenarios are run
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85998DD4-A045-DA44-BBC4-71B1DCA3CB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE701FE4-E370-FD42-ABBD-ED00616B0811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="-18060" windowWidth="25880" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OperationScenario_Component_Bui!$A$1:$P$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">OperationScenario_Component_Bui!$A$1:$P$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>ID_Building</t>
   </si>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,7 +980,7 @@
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -998,10 +998,10 @@
         <v>174.14</v>
       </c>
       <c r="G2" s="1">
-        <v>286.52800000000002</v>
+        <v>303.87599999999998</v>
       </c>
       <c r="H2" s="1">
-        <v>115.621</v>
+        <v>117.355</v>
       </c>
       <c r="I2" s="1">
         <v>49.261000000000003</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -1048,10 +1048,10 @@
         <v>174.14</v>
       </c>
       <c r="G3" s="1">
-        <v>273.15499999999997</v>
+        <v>286.52800000000002</v>
       </c>
       <c r="H3" s="1">
-        <v>114.283</v>
+        <v>115.621</v>
       </c>
       <c r="I3" s="1">
         <v>49.261000000000003</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1098,10 +1098,10 @@
         <v>174.14</v>
       </c>
       <c r="G4" s="1">
-        <v>303.87599999999998</v>
+        <v>274.81700000000001</v>
       </c>
       <c r="H4" s="1">
-        <v>136.28700000000001</v>
+        <v>114.45</v>
       </c>
       <c r="I4" s="1">
         <v>49.261000000000003</v>
@@ -1128,9 +1128,109 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1949</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1957</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>174.14</v>
+      </c>
+      <c r="G5" s="1">
+        <v>273.15499999999997</v>
+      </c>
+      <c r="H5" s="1">
+        <v>114.283</v>
+      </c>
+      <c r="I5" s="1">
+        <v>49.261000000000003</v>
+      </c>
+      <c r="J5" s="1">
+        <v>213505.516</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
+        <v>10.037000000000001</v>
+      </c>
+      <c r="N5" s="1">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1.619</v>
+      </c>
+      <c r="P5" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1949</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1957</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>174.14</v>
+      </c>
+      <c r="G6" s="1">
+        <v>303.87599999999998</v>
+      </c>
+      <c r="H6" s="1">
+        <v>136.28700000000001</v>
+      </c>
+      <c r="I6" s="1">
+        <v>49.261000000000003</v>
+      </c>
+      <c r="J6" s="1">
+        <v>213505.516</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1">
+        <v>10.037000000000001</v>
+      </c>
+      <c r="N6" s="1">
+        <v>4.5330000000000004</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1.619</v>
+      </c>
+      <c r="P6" s="1">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:P4" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
+  <autoFilter ref="A1:P6" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified ID_Buildings - 1, 2, 3 according to efficiency, 1 is the best.
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/Flex/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85998DD4-A045-DA44-BBC4-71B1DCA3CB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2151E15-2CDE-824A-8B50-9B1519B8135C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2120" yWindow="-18060" windowWidth="25880" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,7 +918,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -978,9 +978,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -998,10 +998,10 @@
         <v>174.14</v>
       </c>
       <c r="G2" s="1">
-        <v>286.52800000000002</v>
+        <v>273.15499999999997</v>
       </c>
       <c r="H2" s="1">
-        <v>115.621</v>
+        <v>114.283</v>
       </c>
       <c r="I2" s="1">
         <v>49.261000000000003</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -1048,10 +1048,10 @@
         <v>174.14</v>
       </c>
       <c r="G3" s="1">
-        <v>273.15499999999997</v>
+        <v>286.52800000000002</v>
       </c>
       <c r="H3" s="1">
-        <v>114.283</v>
+        <v>115.621</v>
       </c>
       <c r="I3" s="1">
         <v>49.261000000000003</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
changed the input for the buildings with inner walls
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07AA7E2-EBAA-4B3D-B34F-E63FC3DE0724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3CD551-A72A-402B-995A-39C8E0B390E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
@@ -913,17 +913,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +975,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1000,13 +1002,13 @@
         <v>46.820285138385813</v>
       </c>
       <c r="I2">
-        <v>57.518954565333338</v>
+        <v>59.742655765333339</v>
       </c>
       <c r="J2">
-        <v>3301822.987646373</v>
+        <v>2198880.057077196</v>
       </c>
       <c r="K2">
-        <v>1.535039676655537</v>
+        <v>4.0623860448150264</v>
       </c>
       <c r="L2">
         <v>4.09</v>
@@ -1024,7 +1026,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1051,13 +1053,13 @@
         <v>24.481459292984571</v>
       </c>
       <c r="I3">
-        <v>58.725545181333331</v>
+        <v>60.949246372000012</v>
       </c>
       <c r="J3">
-        <v>1020318.740713089</v>
+        <v>1647301.3903511949</v>
       </c>
       <c r="K3">
-        <v>2.1205248132518739</v>
+        <v>3.8194442353077571</v>
       </c>
       <c r="L3">
         <v>4.09</v>
@@ -1075,7 +1077,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1102,13 +1104,13 @@
         <v>21.10430366673528</v>
       </c>
       <c r="I4">
-        <v>49.14840339733334</v>
+        <v>51.041617349333343</v>
       </c>
       <c r="J4">
-        <v>772431.54974010936</v>
+        <v>1369607.7493062681</v>
       </c>
       <c r="K4">
-        <v>2.3307207238846548</v>
+        <v>4.2169880423676682</v>
       </c>
       <c r="L4">
         <v>4.09</v>
@@ -1126,7 +1128,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1153,13 +1155,13 @@
         <v>37.769176061172537</v>
       </c>
       <c r="I5">
-        <v>58.15579926800001</v>
+        <v>63.527866257333329</v>
       </c>
       <c r="J5">
-        <v>2410581.2112796581</v>
+        <v>3934822.366038735</v>
       </c>
       <c r="K5">
-        <v>1.773353404882656</v>
+        <v>3.9965733530002998</v>
       </c>
       <c r="L5">
         <v>4.09</v>
@@ -1177,7 +1179,7 @@
         <v>21000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1204,13 +1206,13 @@
         <v>21.96151229790096</v>
       </c>
       <c r="I6">
-        <v>58.233763111999998</v>
+        <v>63.605830101333339</v>
       </c>
       <c r="J6">
-        <v>1650933.307061696</v>
+        <v>3415853.5604104698</v>
       </c>
       <c r="K6">
-        <v>1.8449969481345549</v>
+        <v>4.1611748771487864</v>
       </c>
       <c r="L6">
         <v>4.09</v>

</xml_diff>

<commit_message>
updated buildings with MFHs
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3CD551-A72A-402B-995A-39C8E0B390E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38703ED2-E76A-4E06-AA9E-94CDF6DB14BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>ID_Building</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>SFH</t>
+  </si>
+  <si>
+    <t>MFH</t>
   </si>
 </sst>
 </file>
@@ -911,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1193,7 +1196,7 @@
         <v>2008</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f>F6/42.5</f>
         <v>5.2088561576470589</v>
       </c>
       <c r="F6">
@@ -1227,6 +1230,210 @@
         <v>2.709594866848855</v>
       </c>
       <c r="P6">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>2002</v>
+      </c>
+      <c r="D7">
+        <v>2008</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E10" si="1">F7/42.5</f>
+        <v>12.389220717647058</v>
+      </c>
+      <c r="F7">
+        <v>526.54188049999993</v>
+      </c>
+      <c r="G7">
+        <v>545.92182505920346</v>
+      </c>
+      <c r="H7">
+        <v>110.37063172236979</v>
+      </c>
+      <c r="I7">
+        <v>195.04737837333329</v>
+      </c>
+      <c r="J7">
+        <v>1976692.2205915591</v>
+      </c>
+      <c r="K7">
+        <v>3.1881206593694991</v>
+      </c>
+      <c r="L7">
+        <v>4.09</v>
+      </c>
+      <c r="M7">
+        <v>19.985595685714241</v>
+      </c>
+      <c r="N7">
+        <v>9.9927978428571205</v>
+      </c>
+      <c r="O7">
+        <v>9.9927978428571205</v>
+      </c>
+      <c r="P7">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>2002</v>
+      </c>
+      <c r="D8">
+        <v>2008</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>12.389220717647058</v>
+      </c>
+      <c r="F8">
+        <v>526.54188049999993</v>
+      </c>
+      <c r="G8">
+        <v>311.63072655812732</v>
+      </c>
+      <c r="H8">
+        <v>73.936508821704834</v>
+      </c>
+      <c r="I8">
+        <v>192.79152078666669</v>
+      </c>
+      <c r="J8">
+        <v>1825798.5110075211</v>
+      </c>
+      <c r="K8">
+        <v>3.3021848795015778</v>
+      </c>
+      <c r="L8">
+        <v>4.09</v>
+      </c>
+      <c r="M8">
+        <v>18.174420757741562</v>
+      </c>
+      <c r="N8">
+        <v>9.087210378870779</v>
+      </c>
+      <c r="O8">
+        <v>9.087210378870779</v>
+      </c>
+      <c r="P8">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>2002</v>
+      </c>
+      <c r="D9">
+        <v>2008</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>9.1962475294117656</v>
+      </c>
+      <c r="F9">
+        <v>390.84052000000003</v>
+      </c>
+      <c r="G9">
+        <v>715.49033468132347</v>
+      </c>
+      <c r="H9">
+        <v>77.448621722548552</v>
+      </c>
+      <c r="I9">
+        <v>177.82566969333331</v>
+      </c>
+      <c r="J9">
+        <v>3482782.0897382898</v>
+      </c>
+      <c r="K9">
+        <v>3.5556844994939119</v>
+      </c>
+      <c r="L9">
+        <v>4.09</v>
+      </c>
+      <c r="M9">
+        <v>12.228544698146701</v>
+      </c>
+      <c r="N9">
+        <v>6.1142723490733522</v>
+      </c>
+      <c r="O9">
+        <v>6.1142723490733522</v>
+      </c>
+      <c r="P9">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>2002</v>
+      </c>
+      <c r="D10">
+        <v>2008</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>9.1962475294117656</v>
+      </c>
+      <c r="F10">
+        <v>390.84052000000003</v>
+      </c>
+      <c r="G10">
+        <v>363.4430590073618</v>
+      </c>
+      <c r="H10">
+        <v>50.280800635531001</v>
+      </c>
+      <c r="I10">
+        <v>177.96626804666661</v>
+      </c>
+      <c r="J10">
+        <v>3020247.2967746542</v>
+      </c>
+      <c r="K10">
+        <v>3.6954541563476719</v>
+      </c>
+      <c r="L10">
+        <v>4.09</v>
+      </c>
+      <c r="M10">
+        <v>11.250767088751211</v>
+      </c>
+      <c r="N10">
+        <v>5.6253835443756044</v>
+      </c>
+      <c r="O10">
+        <v>5.6253835443756044</v>
+      </c>
+      <c r="P10">
         <v>21000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
separate vehicle profile files uploaded
</commit_message>
<xml_diff>
--- a/data/input_operation/OperationScenario_Component_Building.xlsx
+++ b/data/input_operation/OperationScenario_Component_Building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input_operation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_operation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF46EF5-58AC-4E79-9AAA-B8E75EC77664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2309F49E-2846-6F42-AB12-F8CFEAA353BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="-18060" windowWidth="25875" windowHeight="16665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="-18060" windowWidth="25880" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Component_Bui" sheetId="1" r:id="rId1"/>
@@ -560,53 +560,52 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,7 +621,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -918,20 +917,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="13" max="13" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,166 +983,165 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>1949</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>1957</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>174.14</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <v>273.15499999999997</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <v>114.283</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2">
         <v>49.261000000000003</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2">
         <v>213505.516</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2">
         <v>3</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2">
         <v>3</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2">
         <v>10.037000000000001</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2">
         <v>4.5330000000000004</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2">
         <v>1.619</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2">
         <v>21000</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="Q2">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>1949</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>1957</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>174.14</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3">
         <v>286.52800000000002</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>115.621</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3">
         <v>49.261000000000003</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3">
         <v>213505.516</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3">
         <v>3</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3">
         <v>3</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3">
         <v>10.037000000000001</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3">
         <v>4.5330000000000004</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3">
         <v>1.619</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3">
         <v>21000</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>1949</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4">
         <v>1957</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>174.14</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <v>303.87599999999998</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
         <v>136.28700000000001</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4">
         <v>49.261000000000003</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4">
         <v>213505.516</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4">
         <v>3</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4">
         <v>10.037000000000001</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4">
         <v>4.5330000000000004</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4">
         <v>1.619</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4">
         <v>21000</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:P4" xr:uid="{1B48CFBC-E64D-4A13-BAE3-02D6E7AC7F10}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>